<commit_message>
ppt and documentation added
</commit_message>
<xml_diff>
--- a/Documentation/TableList.xlsx
+++ b/Documentation/TableList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ei11854\Desktop\EvryTechUtsav2020\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB4CA73-F8AB-49EC-AA68-5F56CA734400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F66A31F-85BF-4673-8AA2-6B2587CC0F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{65FB8C8D-360C-42F9-8B97-DB7E0D03C78A}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="C4:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>